<commit_message>
Removed unnecessary code in an effort to clean up and save some space.
</commit_message>
<xml_diff>
--- a/updatedResults.xlsx
+++ b/updatedResults.xlsx
@@ -47,13 +47,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,22 +432,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>1 2 3, 4 5 6</t>
+          <t>2 2 5, 3 5 7, 1 5 10</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Scheduled</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>T1</t>
+          <t>Unscheduable</t>
         </is>
       </c>
     </row>
@@ -460,64 +447,21 @@
           <t>RMS</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
     </row>
-    <row r="3">
-      <c r="C3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>6</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2 2 5, 3 5 7, 1 5 10</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Unscheduable</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1 2 3, 4 5 6</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>Unscheduable</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>EDF</t>
         </is>

</xml_diff>